<commit_message>
Technology & Real Estate
</commit_message>
<xml_diff>
--- a/Companies.xlsx
+++ b/Companies.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danishmak/Documents/FinanceBusinessModels/IDS_789_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8007FF2-F534-4478-8924-AC537B0C1B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4FBA04-6216-3A45-810B-AFABA7AEB141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34455" yWindow="3345" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
   <si>
     <t>Company Name</t>
   </si>
@@ -179,6 +192,69 @@
   </si>
   <si>
     <t>ONEOK, Inc. (OKE)</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
+    <t>SNOW</t>
+  </si>
+  <si>
+    <t>APLD</t>
+  </si>
+  <si>
+    <t>PLD</t>
+  </si>
+  <si>
+    <t>AMT</t>
+  </si>
+  <si>
+    <t>EQR</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>HST</t>
+  </si>
+  <si>
+    <t>AVB</t>
+  </si>
+  <si>
+    <t>ARE</t>
+  </si>
+  <si>
+    <t>INVH</t>
+  </si>
+  <si>
+    <t>PEAK</t>
+  </si>
+  <si>
+    <t>DLR</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
   </si>
 </sst>
 </file>
@@ -546,19 +622,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A22:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -592,7 +668,7 @@
         <v>53.47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -609,7 +685,7 @@
         <v>57.51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -626,7 +702,7 @@
         <v>54.13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -643,7 +719,7 @@
         <v>-8.57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -660,7 +736,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -677,7 +753,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -694,7 +770,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -711,7 +787,7 @@
         <v>33.270000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -728,7 +804,7 @@
         <v>-9.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -745,7 +821,7 @@
         <v>27.59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -762,7 +838,7 @@
         <v>303.51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -779,7 +855,7 @@
         <v>276.95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -796,7 +872,7 @@
         <v>46.37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -813,7 +889,7 @@
         <v>196.37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -830,7 +906,7 @@
         <v>93.38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -847,7 +923,7 @@
         <v>211.02</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -864,7 +940,7 @@
         <v>53.35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -881,7 +957,7 @@
         <v>219.69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -898,7 +974,7 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -915,7 +991,7 @@
         <v>112.82</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -932,7 +1008,7 @@
         <v>159.18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -949,7 +1025,7 @@
         <v>33.35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -966,7 +1042,7 @@
         <v>145.27000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -983,7 +1059,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1000,7 +1076,7 @@
         <v>84.88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1017,7 +1093,7 @@
         <v>675.16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1034,7 +1110,7 @@
         <v>57.09</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1051,7 +1127,7 @@
         <v>50.64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1068,7 +1144,7 @@
         <v>193.29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1085,7 +1161,7 @@
         <v>-7.22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1102,7 +1178,7 @@
         <v>248.45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1119,7 +1195,7 @@
         <v>33.340000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1136,7 +1212,7 @@
         <v>130.32</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -1153,7 +1229,7 @@
         <v>69.11</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1170,7 +1246,7 @@
         <v>182.79</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1187,7 +1263,7 @@
         <v>119.31</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1204,7 +1280,7 @@
         <v>60.29</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1221,7 +1297,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -1238,7 +1314,7 @@
         <v>37.72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1253,6 +1329,329 @@
       </c>
       <c r="E41">
         <v>117.73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42">
+        <v>2.12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42">
+        <v>47.620000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43">
+        <v>0.92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43">
+        <v>16.830000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44">
+        <v>1.26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44">
+        <v>76.72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45">
+        <v>1.08</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45">
+        <v>35.76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46">
+        <v>1.76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46">
+        <v>200.93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>1.29</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47">
+        <v>22.42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48">
+        <v>1.31</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48">
+        <v>36.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49">
+        <v>1.37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49">
+        <v>-17.62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50">
+        <v>1.55</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50">
+        <v>81.98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51">
+        <v>1.01</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52">
+        <v>9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53">
+        <v>0.85</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53">
+        <v>43.37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54">
+        <v>0.68</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54">
+        <v>41.61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56">
+        <v>0.97</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>45.92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57">
+        <v>1.04</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58">
+        <v>0.92</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58">
+        <v>11.15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59">
+        <v>0.75</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59">
+        <v>-10.84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60">
+        <v>0.71</v>
+      </c>
+      <c r="D60" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60">
+        <v>44.269999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated TSR for Consumer Staples & Industrials
</commit_message>
<xml_diff>
--- a/Companies.xlsx
+++ b/Companies.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\DUKE\STUDIES\FALL 2024\IDS 789 - Finance Fundamentals\IDS_789_Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Downloads\IDS_789_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE27597-5D18-4395-98A1-A82D9BB3AC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731BF057-B7B9-434F-B2FF-451E84F03B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$80</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -731,17 +734,17 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:M32"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -775,7 +778,7 @@
         <v>53.47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -792,7 +795,7 @@
         <v>57.51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -809,7 +812,7 @@
         <v>54.13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -826,7 +829,7 @@
         <v>-8.57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -843,7 +846,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -860,7 +863,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -877,7 +880,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -894,7 +897,7 @@
         <v>33.270000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -911,7 +914,7 @@
         <v>-9.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -928,7 +931,7 @@
         <v>27.59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -945,7 +948,7 @@
         <v>303.51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -962,7 +965,7 @@
         <v>276.95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -979,7 +982,7 @@
         <v>46.37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -996,7 +999,7 @@
         <v>196.37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>93.38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>211.02</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>53.35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>219.69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>112.82</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>159.18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>33.35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>145.27000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>84.88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>675.16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>57.09</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>50.64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>193.29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>-7.22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>248.45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>33.340000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>130.32</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>69.11</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>182.79</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>119.31</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>60.29</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>37.72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>117.73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>1236.1100000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>189.72</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>184.85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>159.34</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>2694.8599999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>249.31</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>173.42</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>-47.52</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>-10.57</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>46.400000000000006</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>102.46</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>27.21</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>21.94</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>26.99</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>-22.759999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>80.600000000000009</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
@@ -1776,10 +1779,10 @@
         <v>26</v>
       </c>
       <c r="E61">
-        <v>15.190000000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>74</v>
       </c>
@@ -1793,10 +1796,10 @@
         <v>28</v>
       </c>
       <c r="E62">
-        <v>14.96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>75</v>
       </c>
@@ -1810,10 +1813,10 @@
         <v>29</v>
       </c>
       <c r="E63">
-        <v>6.04</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34.72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>76</v>
       </c>
@@ -1827,10 +1830,10 @@
         <v>26</v>
       </c>
       <c r="E64">
-        <v>12.659999999999998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>77</v>
       </c>
@@ -1844,10 +1847,10 @@
         <v>26</v>
       </c>
       <c r="E65">
-        <v>12.659999999999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>78</v>
       </c>
@@ -1861,10 +1864,10 @@
         <v>95</v>
       </c>
       <c r="E66">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
@@ -1878,10 +1881,10 @@
         <v>29</v>
       </c>
       <c r="E67">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>211.93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>80</v>
       </c>
@@ -1895,10 +1898,10 @@
         <v>29</v>
       </c>
       <c r="E68">
-        <v>15.72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>81</v>
       </c>
@@ -1912,10 +1915,10 @@
         <v>26</v>
       </c>
       <c r="E69">
-        <v>15.45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>82</v>
       </c>
@@ -1929,10 +1932,10 @@
         <v>28</v>
       </c>
       <c r="E70">
-        <v>15.45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>83</v>
       </c>
@@ -1946,10 +1949,10 @@
         <v>26</v>
       </c>
       <c r="E71">
-        <v>11.600000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>84</v>
       </c>
@@ -1963,10 +1966,10 @@
         <v>28</v>
       </c>
       <c r="E72">
-        <v>15.28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>85</v>
       </c>
@@ -1980,10 +1983,10 @@
         <v>27</v>
       </c>
       <c r="E73">
-        <v>15.09</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>86</v>
       </c>
@@ -1997,10 +2000,10 @@
         <v>28</v>
       </c>
       <c r="E74">
-        <v>54.66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84.32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>87</v>
       </c>
@@ -2014,10 +2017,10 @@
         <v>26</v>
       </c>
       <c r="E75">
-        <v>8.36</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>88</v>
       </c>
@@ -2031,10 +2034,10 @@
         <v>29</v>
       </c>
       <c r="E76">
-        <v>17.43</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>89</v>
       </c>
@@ -2048,10 +2051,10 @@
         <v>26</v>
       </c>
       <c r="E77">
-        <v>14.09</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>-51.22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>90</v>
       </c>
@@ -2065,10 +2068,10 @@
         <v>28</v>
       </c>
       <c r="E78">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>91</v>
       </c>
@@ -2082,10 +2085,10 @@
         <v>26</v>
       </c>
       <c r="E79">
-        <v>12.950000000000001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>92</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>26</v>
       </c>
       <c r="E80">
-        <v>12.83</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>